<commit_message>
Ionization_Edges_database.xlsx needs to be corrected
</commit_message>
<xml_diff>
--- a/Ionization_Edges_database.xlsx
+++ b/Ionization_Edges_database.xlsx
@@ -1,15 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="28204"/>
+  <workbookPr filterPrivacy="1"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/veersaysit/Dropbox/Matlab/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="122211" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -1727,9 +1740,9 @@
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -1762,9 +1775,9 @@
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -1971,12 +1984,12 @@
   <dimension ref="A1:I83"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="M45" sqref="M45"/>
+      <selection activeCell="H52" sqref="H52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>259</v>
       </c>
@@ -2003,7 +2016,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>2</v>
       </c>
@@ -2020,7 +2033,7 @@
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
     </row>
-    <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>3</v>
       </c>
@@ -2037,7 +2050,7 @@
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
     </row>
-    <row r="4" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>4</v>
       </c>
@@ -2054,7 +2067,7 @@
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
     </row>
-    <row r="5" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>5</v>
       </c>
@@ -2071,7 +2084,7 @@
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
     </row>
-    <row r="6" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>6</v>
       </c>
@@ -2088,7 +2101,7 @@
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
     </row>
-    <row r="7" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>7</v>
       </c>
@@ -2105,7 +2118,7 @@
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
     </row>
-    <row r="8" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>8</v>
       </c>
@@ -2122,7 +2135,7 @@
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
     </row>
-    <row r="9" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>9</v>
       </c>
@@ -2139,7 +2152,7 @@
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
     </row>
-    <row r="10" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>10</v>
       </c>
@@ -2158,7 +2171,7 @@
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
     </row>
-    <row r="11" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>11</v>
       </c>
@@ -2177,7 +2190,7 @@
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
     </row>
-    <row r="12" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>12</v>
       </c>
@@ -2196,7 +2209,7 @@
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
     </row>
-    <row r="13" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>13</v>
       </c>
@@ -2217,7 +2230,7 @@
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
     </row>
-    <row r="14" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>14</v>
       </c>
@@ -2238,7 +2251,7 @@
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
     </row>
-    <row r="15" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>15</v>
       </c>
@@ -2259,7 +2272,7 @@
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
     </row>
-    <row r="16" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>16</v>
       </c>
@@ -2280,7 +2293,7 @@
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
     </row>
-    <row r="17" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>17</v>
       </c>
@@ -2301,7 +2314,7 @@
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
     </row>
-    <row r="18" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>18</v>
       </c>
@@ -2322,7 +2335,7 @@
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
     </row>
-    <row r="19" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>19</v>
       </c>
@@ -2343,7 +2356,7 @@
       <c r="H19" s="3"/>
       <c r="I19" s="3"/>
     </row>
-    <row r="20" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>20</v>
       </c>
@@ -2366,7 +2379,7 @@
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
     </row>
-    <row r="21" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>21</v>
       </c>
@@ -2389,7 +2402,7 @@
       <c r="H21" s="3"/>
       <c r="I21" s="3"/>
     </row>
-    <row r="22" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>22</v>
       </c>
@@ -2414,7 +2427,7 @@
       <c r="H22" s="3"/>
       <c r="I22" s="3"/>
     </row>
-    <row r="23" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>23</v>
       </c>
@@ -2439,7 +2452,7 @@
       <c r="H23" s="3"/>
       <c r="I23" s="3"/>
     </row>
-    <row r="24" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>24</v>
       </c>
@@ -2464,7 +2477,7 @@
       <c r="H24" s="3"/>
       <c r="I24" s="3"/>
     </row>
-    <row r="25" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>25</v>
       </c>
@@ -2489,7 +2502,7 @@
       <c r="H25" s="3"/>
       <c r="I25" s="3"/>
     </row>
-    <row r="26" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>26</v>
       </c>
@@ -2514,7 +2527,7 @@
       <c r="H26" s="3"/>
       <c r="I26" s="3"/>
     </row>
-    <row r="27" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>27</v>
       </c>
@@ -2539,7 +2552,7 @@
       <c r="H27" s="3"/>
       <c r="I27" s="3"/>
     </row>
-    <row r="28" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>28</v>
       </c>
@@ -2564,7 +2577,7 @@
       <c r="H28" s="3"/>
       <c r="I28" s="3"/>
     </row>
-    <row r="29" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>29</v>
       </c>
@@ -2589,7 +2602,7 @@
       <c r="H29" s="3"/>
       <c r="I29" s="3"/>
     </row>
-    <row r="30" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>30</v>
       </c>
@@ -2614,7 +2627,7 @@
       <c r="H30" s="3"/>
       <c r="I30" s="3"/>
     </row>
-    <row r="31" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>31</v>
       </c>
@@ -2637,7 +2650,7 @@
       <c r="H31" s="3"/>
       <c r="I31" s="3"/>
     </row>
-    <row r="32" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>32</v>
       </c>
@@ -2662,7 +2675,7 @@
       </c>
       <c r="I32" s="3"/>
     </row>
-    <row r="33" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>33</v>
       </c>
@@ -2687,7 +2700,7 @@
       </c>
       <c r="I33" s="3"/>
     </row>
-    <row r="34" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>34</v>
       </c>
@@ -2712,7 +2725,7 @@
       </c>
       <c r="I34" s="3"/>
     </row>
-    <row r="35" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>35</v>
       </c>
@@ -2737,7 +2750,7 @@
       </c>
       <c r="I35" s="3"/>
     </row>
-    <row r="36" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>36</v>
       </c>
@@ -2762,7 +2775,7 @@
       </c>
       <c r="I36" s="3"/>
     </row>
-    <row r="37" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>37</v>
       </c>
@@ -2787,7 +2800,7 @@
       </c>
       <c r="I37" s="3"/>
     </row>
-    <row r="38" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>38</v>
       </c>
@@ -2814,7 +2827,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="39" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>39</v>
       </c>
@@ -2841,7 +2854,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="40" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>40</v>
       </c>
@@ -2868,7 +2881,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="41" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>41</v>
       </c>
@@ -2895,7 +2908,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="42" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>42</v>
       </c>
@@ -2922,7 +2935,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>44</v>
       </c>
@@ -2949,7 +2962,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="44" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>45</v>
       </c>
@@ -2970,7 +2983,7 @@
       <c r="H44" s="3"/>
       <c r="I44" s="3"/>
     </row>
-    <row r="45" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>46</v>
       </c>
@@ -2991,7 +3004,7 @@
       <c r="H45" s="3"/>
       <c r="I45" s="3"/>
     </row>
-    <row r="46" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>47</v>
       </c>
@@ -3012,7 +3025,7 @@
       <c r="H46" s="3"/>
       <c r="I46" s="3"/>
     </row>
-    <row r="47" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>48</v>
       </c>
@@ -3033,7 +3046,7 @@
       <c r="H47" s="3"/>
       <c r="I47" s="3"/>
     </row>
-    <row r="48" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>49</v>
       </c>
@@ -3054,7 +3067,7 @@
       <c r="H48" s="3"/>
       <c r="I48" s="3"/>
     </row>
-    <row r="49" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>50</v>
       </c>
@@ -3075,7 +3088,7 @@
       <c r="H49" s="3"/>
       <c r="I49" s="3"/>
     </row>
-    <row r="50" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>51</v>
       </c>
@@ -3098,7 +3111,7 @@
       <c r="H50" s="3"/>
       <c r="I50" s="3"/>
     </row>
-    <row r="51" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>52</v>
       </c>
@@ -3121,7 +3134,7 @@
       <c r="H51" s="3"/>
       <c r="I51" s="3"/>
     </row>
-    <row r="52" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>53</v>
       </c>
@@ -3144,7 +3157,7 @@
       <c r="H52" s="3"/>
       <c r="I52" s="3"/>
     </row>
-    <row r="53" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>54</v>
       </c>
@@ -3167,7 +3180,7 @@
       <c r="H53" s="3"/>
       <c r="I53" s="3"/>
     </row>
-    <row r="54" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>55</v>
       </c>
@@ -3188,7 +3201,7 @@
       <c r="H54" s="3"/>
       <c r="I54" s="3"/>
     </row>
-    <row r="55" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <v>56</v>
       </c>
@@ -3209,7 +3222,7 @@
       <c r="H55" s="3"/>
       <c r="I55" s="3"/>
     </row>
-    <row r="56" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>57</v>
       </c>
@@ -3230,7 +3243,7 @@
       <c r="H56" s="3"/>
       <c r="I56" s="3"/>
     </row>
-    <row r="57" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <v>58</v>
       </c>
@@ -3251,7 +3264,7 @@
       <c r="H57" s="3"/>
       <c r="I57" s="3"/>
     </row>
-    <row r="58" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <v>59</v>
       </c>
@@ -3272,7 +3285,7 @@
       <c r="H58" s="3"/>
       <c r="I58" s="3"/>
     </row>
-    <row r="59" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <v>60</v>
       </c>
@@ -3293,7 +3306,7 @@
       <c r="H59" s="3"/>
       <c r="I59" s="3"/>
     </row>
-    <row r="60" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
         <v>62</v>
       </c>
@@ -3314,7 +3327,7 @@
       <c r="H60" s="3"/>
       <c r="I60" s="3"/>
     </row>
-    <row r="61" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
         <v>63</v>
       </c>
@@ -3335,7 +3348,7 @@
       <c r="H61" s="3"/>
       <c r="I61" s="3"/>
     </row>
-    <row r="62" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
         <v>64</v>
       </c>
@@ -3356,7 +3369,7 @@
       <c r="H62" s="3"/>
       <c r="I62" s="3"/>
     </row>
-    <row r="63" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
         <v>65</v>
       </c>
@@ -3377,7 +3390,7 @@
       <c r="H63" s="3"/>
       <c r="I63" s="3"/>
     </row>
-    <row r="64" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
         <v>66</v>
       </c>
@@ -3400,7 +3413,7 @@
       </c>
       <c r="I64" s="3"/>
     </row>
-    <row r="65" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
         <v>67</v>
       </c>
@@ -3423,7 +3436,7 @@
       </c>
       <c r="I65" s="3"/>
     </row>
-    <row r="66" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
         <v>68</v>
       </c>
@@ -3446,7 +3459,7 @@
       </c>
       <c r="I66" s="3"/>
     </row>
-    <row r="67" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
         <v>69</v>
       </c>
@@ -3469,7 +3482,7 @@
       </c>
       <c r="I67" s="3"/>
     </row>
-    <row r="68" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
         <v>70</v>
       </c>
@@ -3492,7 +3505,7 @@
       </c>
       <c r="I68" s="3"/>
     </row>
-    <row r="69" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
         <v>71</v>
       </c>
@@ -3515,7 +3528,7 @@
       </c>
       <c r="I69" s="3"/>
     </row>
-    <row r="70" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
         <v>72</v>
       </c>
@@ -3536,7 +3549,7 @@
       </c>
       <c r="I70" s="3"/>
     </row>
-    <row r="71" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
         <v>73</v>
       </c>
@@ -3557,7 +3570,7 @@
       </c>
       <c r="I71" s="3"/>
     </row>
-    <row r="72" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
         <v>74</v>
       </c>
@@ -3580,7 +3593,7 @@
       </c>
       <c r="I72" s="3"/>
     </row>
-    <row r="73" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A73" s="1">
         <v>75</v>
       </c>
@@ -3603,7 +3616,7 @@
       </c>
       <c r="I73" s="3"/>
     </row>
-    <row r="74" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
         <v>76</v>
       </c>
@@ -3626,7 +3639,7 @@
       </c>
       <c r="I74" s="3"/>
     </row>
-    <row r="75" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
         <v>77</v>
       </c>
@@ -3649,7 +3662,7 @@
       </c>
       <c r="I75" s="3"/>
     </row>
-    <row r="76" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
         <v>78</v>
       </c>
@@ -3672,7 +3685,7 @@
       </c>
       <c r="I76" s="3"/>
     </row>
-    <row r="77" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
         <v>79</v>
       </c>
@@ -3695,7 +3708,7 @@
       </c>
       <c r="I77" s="3"/>
     </row>
-    <row r="78" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A78" s="1">
         <v>80</v>
       </c>
@@ -3716,7 +3729,7 @@
       </c>
       <c r="I78" s="3"/>
     </row>
-    <row r="79" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A79" s="1">
         <v>81</v>
       </c>
@@ -3737,7 +3750,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="80" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
         <v>82</v>
       </c>
@@ -3758,7 +3771,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="81" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A81" s="1">
         <v>83</v>
       </c>
@@ -3779,7 +3792,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="82" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A82" s="1">
         <v>90</v>
       </c>
@@ -3800,7 +3813,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="83" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A83" s="1">
         <v>92</v>
       </c>

</xml_diff>

<commit_message>
Trying new methods for edge_detection
</commit_message>
<xml_diff>
--- a/Ionization_Edges_database.xlsx
+++ b/Ionization_Edges_database.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="28204"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="28629"/>
   <workbookPr filterPrivacy="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -1983,8 +1983,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="H52" sqref="H52"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="K64" sqref="K64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>